<commit_message>
main screipt + streamlit base + reqs
</commit_message>
<xml_diff>
--- a/data/CB/otchet.xlsx
+++ b/data/CB/otchet.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danilalipatov/Ratings-analysis-project/data/CB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EBEC37-A2A1-9F45-BF30-36BB61200186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A08910D-35C2-704B-849C-5BEB3A1E6B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2680" yWindow="1600" windowWidth="28240" windowHeight="17240" xr2:uid="{2B38557D-B60E-ED45-A053-49C28265D2ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -521,7 +521,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>